<commit_message>
update sampai sebelum ppd cetak
</commit_message>
<xml_diff>
--- a/public/report/KOMITE.xlsx
+++ b/public/report/KOMITE.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\golang\src\github.com\bbliong\sim-bmm\public\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E57E69-78B4-4366-BD50-6396D092AA5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22FD7DE-182A-4288-B136-A15B785C3650}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5E293F62-818E-4F82-94B0-C70CFD483C1D}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{5E293F62-818E-4F82-94B0-C70CFD483C1D}"/>
   </bookViews>
   <sheets>
     <sheet name="KOMITE ORIGINAL level 1" sheetId="1" r:id="rId1"/>
     <sheet name="KOMITE ORIGINAL level 2" sheetId="3" r:id="rId2"/>
-    <sheet name="KOMITE ORIGINAL level 3 " sheetId="4" r:id="rId3"/>
+    <sheet name="KOMITE ORIGINAL level 3" sheetId="4" r:id="rId3"/>
     <sheet name="KOMITE ORIGINAL level 4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -448,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -769,18 +769,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -793,6 +805,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -804,27 +819,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1459,7 +1453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8268F91-EE55-4413-BB97-E80ACBF28EEE}">
   <dimension ref="B1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="52" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="52" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
@@ -2995,8 +2989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63519976-8819-4168-9A23-C8073530CACA}">
   <dimension ref="B1:P57"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="52" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29:J30"/>
+    <sheetView topLeftCell="A22" zoomScale="52" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3445,8 +3439,8 @@
       <c r="J34" s="97"/>
     </row>
     <row r="35" spans="2:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="114"/>
-      <c r="C35" s="115"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="98"/>
       <c r="D35" s="47"/>
       <c r="E35" s="63" t="s">
         <v>50</v>
@@ -3460,26 +3454,26 @@
       <c r="J35" s="64"/>
     </row>
     <row r="36" spans="2:10" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="116"/>
-      <c r="C36" s="117"/>
+      <c r="B36" s="88"/>
+      <c r="C36" s="113"/>
       <c r="D36" s="47"/>
       <c r="E36" s="114"/>
       <c r="F36" s="115"/>
-      <c r="G36" s="128"/>
-      <c r="H36" s="129"/>
-      <c r="I36" s="129"/>
-      <c r="J36" s="130"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="119"/>
+      <c r="I36" s="119"/>
+      <c r="J36" s="120"/>
     </row>
     <row r="37" spans="2:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="118"/>
-      <c r="C37" s="119"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="99"/>
       <c r="D37" s="47"/>
-      <c r="E37" s="118"/>
-      <c r="F37" s="119"/>
-      <c r="G37" s="131"/>
-      <c r="H37" s="132"/>
-      <c r="I37" s="132"/>
-      <c r="J37" s="133"/>
+      <c r="E37" s="116"/>
+      <c r="F37" s="117"/>
+      <c r="G37" s="121"/>
+      <c r="H37" s="122"/>
+      <c r="I37" s="122"/>
+      <c r="J37" s="123"/>
     </row>
     <row r="38" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="86"/>
@@ -4211,52 +4205,52 @@
       <c r="J33" s="99"/>
     </row>
     <row r="34" spans="2:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="120" t="s">
+      <c r="B34" s="124" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="121"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="121"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="121"/>
-      <c r="H34" s="121"/>
-      <c r="I34" s="121"/>
-      <c r="J34" s="122"/>
+      <c r="C34" s="125"/>
+      <c r="D34" s="125"/>
+      <c r="E34" s="125"/>
+      <c r="F34" s="125"/>
+      <c r="G34" s="125"/>
+      <c r="H34" s="125"/>
+      <c r="I34" s="125"/>
+      <c r="J34" s="126"/>
     </row>
     <row r="35" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="123"/>
-      <c r="C35" s="123"/>
+      <c r="B35" s="127"/>
+      <c r="C35" s="127"/>
       <c r="D35" s="46"/>
-      <c r="E35" s="124" t="s">
+      <c r="E35" s="129" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="124"/>
-      <c r="G35" s="125"/>
-      <c r="H35" s="126"/>
-      <c r="I35" s="126"/>
-      <c r="J35" s="127"/>
+      <c r="F35" s="129"/>
+      <c r="G35" s="130"/>
+      <c r="H35" s="131"/>
+      <c r="I35" s="131"/>
+      <c r="J35" s="132"/>
     </row>
     <row r="36" spans="2:10" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="123"/>
-      <c r="C36" s="123"/>
+      <c r="B36" s="127"/>
+      <c r="C36" s="127"/>
       <c r="D36" s="46"/>
-      <c r="E36" s="123"/>
-      <c r="F36" s="123"/>
-      <c r="G36" s="134"/>
-      <c r="H36" s="134"/>
-      <c r="I36" s="134"/>
-      <c r="J36" s="134"/>
+      <c r="E36" s="127"/>
+      <c r="F36" s="127"/>
+      <c r="G36" s="128"/>
+      <c r="H36" s="128"/>
+      <c r="I36" s="128"/>
+      <c r="J36" s="128"/>
     </row>
     <row r="37" spans="2:10" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="123"/>
-      <c r="C37" s="123"/>
+      <c r="B37" s="127"/>
+      <c r="C37" s="127"/>
       <c r="D37" s="46"/>
-      <c r="E37" s="123"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="134"/>
-      <c r="H37" s="134"/>
-      <c r="I37" s="134"/>
-      <c r="J37" s="134"/>
+      <c r="E37" s="127"/>
+      <c r="F37" s="127"/>
+      <c r="G37" s="128"/>
+      <c r="H37" s="128"/>
+      <c r="I37" s="128"/>
+      <c r="J37" s="128"/>
     </row>
     <row r="38" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="88"/>
@@ -4515,8 +4509,6 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="F57:G57"/>
     <mergeCell ref="C58:E58"/>
     <mergeCell ref="F58:G58"/>
     <mergeCell ref="B35:C37"/>
@@ -4531,31 +4523,28 @@
     <mergeCell ref="C56:E56"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="B41:D43"/>
-    <mergeCell ref="B31:D33"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="B34:J34"/>
-    <mergeCell ref="B38:D40"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="G38:J38"/>
     <mergeCell ref="E39:F40"/>
     <mergeCell ref="G39:J40"/>
-    <mergeCell ref="B28:D30"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="E29:F30"/>
+    <mergeCell ref="B31:D33"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:J31"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:J23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:J24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B27:J27"/>
-    <mergeCell ref="E29:F30"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:J22"/>
     <mergeCell ref="B18:C20"/>
     <mergeCell ref="E18:J18"/>
     <mergeCell ref="E19:F19"/>
@@ -4593,6 +4582,11 @@
     <mergeCell ref="B48:D50"/>
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="G48:J48"/>
+    <mergeCell ref="B28:D30"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B38:D40"/>
   </mergeCells>
   <pageMargins left="0.28000000000000003" right="0.03" top="0.19" bottom="0.12" header="0.12" footer="0.12"/>
   <pageSetup paperSize="9" scale="66" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>